<commit_message>
correccion de logs, registra guia
</commit_message>
<xml_diff>
--- a/plantilla.xlsx
+++ b/plantilla.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Sistema_control_canal\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18915" windowHeight="6480"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>verde</t>
   </si>
@@ -41,16 +36,16 @@
     <t>canal</t>
   </si>
   <si>
-    <t>amarillo</t>
+    <t>rojo</t>
   </si>
   <si>
-    <t>rojo</t>
+    <t>amarillo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,11 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,7 +184,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,16 +422,16 @@
       <c r="A2">
         <v>100</v>
       </c>
-      <c r="B2">
-        <v>135</v>
+      <c r="B2" s="2">
+        <v>101</v>
       </c>
       <c r="C2" s="1">
-        <v>45769</v>
-      </c>
-      <c r="D2" s="3">
+        <v>45770</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -443,142 +439,78 @@
       <c r="A3">
         <v>100</v>
       </c>
-      <c r="B3" s="3">
-        <v>136</v>
+      <c r="B3" s="2">
+        <v>102</v>
       </c>
       <c r="C3" s="1">
-        <v>45769</v>
-      </c>
-      <c r="E3" t="s">
+        <v>45770</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>137</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>100</v>
-      </c>
-      <c r="B5" s="3">
-        <v>138</v>
-      </c>
-      <c r="C5" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>100</v>
-      </c>
-      <c r="B6">
-        <v>139</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>100</v>
-      </c>
-      <c r="B7" s="3">
-        <v>140</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>100</v>
-      </c>
-      <c r="B8">
-        <v>141</v>
-      </c>
-      <c r="C8" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>100</v>
-      </c>
-      <c r="B9" s="3">
-        <v>142</v>
-      </c>
-      <c r="C9" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>100</v>
-      </c>
-      <c r="B10">
-        <v>143</v>
-      </c>
-      <c r="C10" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>100</v>
-      </c>
-      <c r="B11" s="3">
-        <v>144</v>
-      </c>
-      <c r="C11" s="1">
-        <v>45769</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -586,6 +518,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -603,6 +536,38 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -612,12 +577,247 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>100</v>
+      </c>
+      <c r="B1" s="2">
+        <v>103</v>
+      </c>
+      <c r="C1" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2">
+        <v>104</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="2">
+        <v>105</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="2">
+        <v>106</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5" s="2">
+        <v>107</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6" s="2">
+        <v>108</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8" s="2">
+        <v>110</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9" s="2">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10" s="2">
+        <v>112</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11" s="2">
+        <v>113</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45770</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12" s="2">
+        <v>114</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45770</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13" s="2">
+        <v>115</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45770</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14" s="2">
+        <v>116</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45770</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="B15" s="2">
+        <v>117</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45770</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>